<commit_message>
refactor write_t_excel code docs data
</commit_message>
<xml_diff>
--- a/inst/results/here_1.0.1/here_1.0.1.tm_doc.xlsx
+++ b/inst/results/here_1.0.1/here_1.0.1.tm_doc.xlsx
@@ -12,9 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">package_function</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">Traceability Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-07 12:26:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exported_function</t>
   </si>
   <si>
     <t xml:space="preserve">code_script</t>
@@ -23,37 +38,31 @@
     <t xml:space="preserve">documentation</t>
   </si>
   <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
     <t xml:space="preserve">coverage_percent</t>
   </si>
   <si>
-    <t xml:space="preserve">date_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">here</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-06-06 15:44:02</t>
-  </si>
-  <si>
     <t xml:space="preserve">dr_here</t>
   </si>
   <si>
     <t xml:space="preserve">R/dr_here.R</t>
   </si>
   <si>
-    <t xml:space="preserve">man/dr_here.Rd</t>
+    <t xml:space="preserve">dr_here.Rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dr_here() shows a message that by default also includes thereason why here() is set to a particular directory.Use this function if here() gives unexpected results.</t>
   </si>
   <si>
     <t xml:space="preserve">R/here.R</t>
   </si>
   <si>
-    <t xml:space="preserve">man/here.Rd</t>
+    <t xml:space="preserve">here.Rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">here() uses a reasonable heuristics to find your project's files, based onthe current working directory at the time when the package is loaded.Use it as a drop-in replacement for file.path(), it will always locate thefiles relative to your project root.</t>
   </si>
   <si>
     <t xml:space="preserve">i_am</t>
@@ -62,7 +71,10 @@
     <t xml:space="preserve">R/i_am.R</t>
   </si>
   <si>
-    <t xml:space="preserve">man/i_am.Rd</t>
+    <t xml:space="preserve">i_am.Rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add a call to here::i_am("&lt;project-relative path&gt;.&lt;ext&gt;")at the top of your R script or in the first chunk of your rmarkdown document.This ensures that the project root is set up correctly:subsequent calls to here() will refer to the implied project root.If the current working directory is outside of the projectwhere the script or report is intended to run, it will failwith a descriptive message.</t>
   </si>
   <si>
     <t xml:space="preserve">set_here</t>
@@ -71,7 +83,10 @@
     <t xml:space="preserve">R/set_here.R</t>
   </si>
   <si>
-    <t xml:space="preserve">man/set_here.Rd</t>
+    <t xml:space="preserve">set_here.Rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">html&lt;a href='https://www.tidyverse.org/lifecycle/#superseded'&gt;&lt;img src='figures/lifecycle-superseded.svg' alt='Superseded lifecycle'&gt;&lt;/a&gt;Superseded</t>
   </si>
 </sst>
 </file>
@@ -422,132 +437,113 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="18.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="19.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="14.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="17.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="18.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="21.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="15.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="401.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="18.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="n">
         <v>100</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="n">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="n">
         <v>100</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="n">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="n">
         <v>95.83</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="n">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="n">
         <v>100</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>